<commit_message>
SO DONE WITH 2D
</commit_message>
<xml_diff>
--- a/SystemsWorld/Tex/2DprojectSW_F06_T06_Q3.xlsx
+++ b/SystemsWorld/Tex/2DprojectSW_F06_T06_Q3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Lazykid/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SUTD Term 3\2D\green-fingers-2d\SystemsWorld\Tex\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -52,11 +52,11 @@
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="sum_of_x_i">Q.3b!$F$14</definedName>
     <definedName name="x_i">Q.3b!$F$3:$F$12</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -89,6 +89,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>chi square</t>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -144,6 +145,7 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -151,6 +153,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -527,12 +530,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -570,19 +576,18 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> chi square </a:t>
+              <a:t> Chi Squared against</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>vs order </a:t>
+              <a:t> Order of Controller</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -615,14 +620,14 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="15875" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -634,71 +639,97 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:val>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Q.3b!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Q.3b!$H$17:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.152</c:v>
+                  <c:v>1.1519999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B76E-4F66-B2C9-37EB3D6C4686}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="-1030458944"/>
-        <c:axId val="-1109415136"/>
-      </c:lineChart>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -718,6 +749,218 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.8506631738166118E-2"/>
+                  <c:y val="-2.0166984255578349E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.5751286815753988E-2"/>
+                  <c:y val="-0.15483740755547026"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.575128681575396E-2"/>
+                  <c:y val="-0.16381543577546304"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.5751286815754058E-2"/>
+                  <c:y val="-0.16381543577546312"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.575128681575396E-2"/>
+                  <c:y val="-0.15483740755547035"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.2208368601154361E-2"/>
+                  <c:y val="-0.12341430878549554"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.7012997016061505E-2"/>
+                  <c:y val="-0.19972754865543432"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-B76E-4F66-B2C9-37EB3D6C4686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Q.3b!$B$3:$B$12</c:f>
@@ -725,34 +968,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,39 +1007,44 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>20.260716592448</c:v>
+                  <c:v>20.260716592447999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.089836450794126</c:v>
+                  <c:v>3.0898364507941261</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00675415550326038</c:v>
+                  <c:v>6.7541555032603834E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00671634589102055</c:v>
+                  <c:v>6.7163458910205493E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00649321662431249</c:v>
+                  <c:v>6.4932166243124876E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00510206909265717</c:v>
+                  <c:v>5.1020690926571743E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00312269168145197</c:v>
+                  <c:v>3.1226916814519729E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00272772690885927</c:v>
+                  <c:v>2.7277269088592658E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.000374947305434904</c:v>
+                  <c:v>3.7494730543490392E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9664382831248E-11</c:v>
+                  <c:v>4.9664382831247998E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B76E-4F66-B2C9-37EB3D6C4686}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -809,10 +1057,11 @@
         <c:axId val="-1030458944"/>
         <c:axId val="-1109415136"/>
       </c:scatterChart>
-      <c:catAx>
+      <c:valAx>
         <c:axId val="-1030458944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -830,6 +1079,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -851,12 +1114,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>order</a:t>
+                  <a:t>Order of Controller</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -925,11 +1187,8 @@
         </c:txPr>
         <c:crossAx val="-1109415136"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="-1109415136"/>
         <c:scaling>
@@ -951,6 +1210,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -974,7 +1247,7 @@
                   <a:rPr lang="en-GB" sz="1000" b="0" i="1" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>chi square</a:t>
+                  <a:t>Chi  Squared Value</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -986,7 +1259,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1016,6 +1288,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1054,7 +1327,7 @@
         </c:txPr>
         <c:crossAx val="-1030458944"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1662,19 +1935,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>733036</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>4233</xdr:rowOff>
+      <xdr:colOff>744177</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>197333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>358720</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>140591</xdr:rowOff>
+      <xdr:colOff>668421</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>18567</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1691,26 +1970,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>278508</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>100263</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>772365</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>735262</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>189386</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>71738</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>103538</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2751666" y="4912895"/>
-          <a:ext cx="456754" cy="89123"/>
+          <a:off x="772365" y="4964241"/>
+          <a:ext cx="923433" cy="292418"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1739,8 +2024,8 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="800"/>
-            <a:t>1.152</a:t>
+            <a:rPr lang="en-US" sz="900"/>
+            <a:t> 1.152 -</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2015,18 +2300,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
         <v>0</v>
       </c>
@@ -2051,11 +2336,11 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f>C3*F3</f>
+        <f t="shared" ref="H3:H12" si="0">C3*F3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>1</v>
       </c>
@@ -2066,11 +2351,11 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>C4*F4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
         <v>2</v>
       </c>
@@ -2081,11 +2366,11 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <f>C5*F5</f>
+        <f t="shared" si="0"/>
         <v>6.7541555032603834E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6">
         <v>3</v>
       </c>
@@ -2096,11 +2381,11 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f>C6*F6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
         <v>4</v>
       </c>
@@ -2111,11 +2396,11 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <f>C7*F7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>5</v>
       </c>
@@ -2126,11 +2411,11 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <f>C8*F8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>6</v>
       </c>
@@ -2141,11 +2426,11 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <f>C9*F9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10">
         <v>7</v>
       </c>
@@ -2156,11 +2441,11 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <f>C10*F10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <v>8</v>
       </c>
@@ -2171,11 +2456,11 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <f>C11*F11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12">
         <v>9</v>
       </c>
@@ -2186,11 +2471,11 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <f>C12*F12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="E14" t="s">
         <v>5</v>
       </c>
@@ -2206,57 +2491,57 @@
         <v>6.7541555032603834E-3</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H17">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H18">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H19">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H20">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H21">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H22">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H23">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H24">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H25">
         <v>1.1519999999999999</v>
       </c>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.55000000000000004">
       <c r="H26">
         <v>1.1519999999999999</v>
       </c>

</xml_diff>